<commit_message>
Updated mapping spreadsheet document attachment metadata
</commit_message>
<xml_diff>
--- a/shared/ojb-resources-common/src/main/resources/ssp/Court_Case_Filing/artifacts/service_model/information_model/IEPD/documentation/impl-artifacts/alaska/AlaskaCriminalCaseMapping.xlsx
+++ b/shared/ojb-resources-common/src/main/resources/ssp/Court_Case_Filing/artifacts/service_model/information_model/IEPD/documentation/impl-artifacts/alaska/AlaskaCriminalCaseMapping.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="5460" windowWidth="28800" windowHeight="18000"/>
+    <workbookView xWindow="-28800" yWindow="5460" windowWidth="24240" windowHeight="13740" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Court Case Filing" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="381">
   <si>
     <t>ATN [Arrest Tracking Number]</t>
   </si>
@@ -1014,6 +1014,156 @@
   <si>
     <t xml:space="preserve">/core:CoreFilingMessage/criminalcase:CriminalCase/j:CaseAugmentation/j:CaseProsecutionAttorney/ecf:EntityPersonnc:PersonName/nc:RoleOfPersonReference
 </t>
+  </si>
+  <si>
+    <t>Document Attachment</t>
+  </si>
+  <si>
+    <t>Document Category</t>
+  </si>
+  <si>
+    <t>Information</t>
+  </si>
+  <si>
+    <t>Document Title</t>
+  </si>
+  <si>
+    <t>District Court for the Third Judicial District at Anchorage</t>
+  </si>
+  <si>
+    <t>Original Complaint Agency ORI</t>
+  </si>
+  <si>
+    <t>Original Complaint Agency ID</t>
+  </si>
+  <si>
+    <t>13-55498</t>
+  </si>
+  <si>
+    <t>Case Tracking Number</t>
+  </si>
+  <si>
+    <t>3AN-14</t>
+  </si>
+  <si>
+    <t>Court Docket Number</t>
+  </si>
+  <si>
+    <t>3AN-14-459-CR</t>
+  </si>
+  <si>
+    <t>Document Key Words</t>
+  </si>
+  <si>
+    <t>Information, Alaska Police Department</t>
+  </si>
+  <si>
+    <t>Document Description</t>
+  </si>
+  <si>
+    <t>Municipality of Anchorage vs Randall James Ferguson</t>
+  </si>
+  <si>
+    <t>Document Creator</t>
+  </si>
+  <si>
+    <t>Cynthia Dubell</t>
+  </si>
+  <si>
+    <t>Document Publisher</t>
+  </si>
+  <si>
+    <t>Municipality of Anchorage</t>
+  </si>
+  <si>
+    <t>Document Media Type</t>
+  </si>
+  <si>
+    <t>Portable Document Format</t>
+  </si>
+  <si>
+    <t>Document Format</t>
+  </si>
+  <si>
+    <t>pdf</t>
+  </si>
+  <si>
+    <t>Document Language</t>
+  </si>
+  <si>
+    <t>en</t>
+  </si>
+  <si>
+    <t>image of signature</t>
+  </si>
+  <si>
+    <t>/cc-filing-doc:CourtCaseFilingDocument/cfd-ext:CourtCaseFilingAttachment/xop:Include/@href</t>
+  </si>
+  <si>
+    <t>/cc-filing-doc:CourtCaseFilingDocument/nc:DocumentCategoryText</t>
+  </si>
+  <si>
+    <t>/cc-filing-doc:CourtCaseFilingDocument/nc:DocumentTitleText</t>
+  </si>
+  <si>
+    <t>/cc-filing-doc:CourtCaseFilingDocument/nc:DocumentKeywordText</t>
+  </si>
+  <si>
+    <t>/cc-filing-doc:CourtCaseFilingDocument/nc:DocumentDescriptionText</t>
+  </si>
+  <si>
+    <t>/cc-filing-doc:CourtCaseFilingDocument/nc:DocumentAuthor/nc:EntityPerson</t>
+  </si>
+  <si>
+    <t>/cc-filing-doc:CourtCaseFilingDocument/nc:PublisherName/nc:EntityPerson</t>
+  </si>
+  <si>
+    <t>/cc-filing-doc:CourtCaseFilingDocument/nc:DocumentMediaCategoryText</t>
+  </si>
+  <si>
+    <t>/cc-filing-doc:CourtCaseFilingDocument/nc:DocumentFormatText</t>
+  </si>
+  <si>
+    <t>/cc-filing-doc:CourtCaseFilingDocument/nc:DocumentLanguageCode</t>
+  </si>
+  <si>
+    <t>/cc-filing-doc:CourtCaseFilingDocument/nc:Person/nc:PersonDigitizedSignatureImage/nc:Base64BinaryObject</t>
+  </si>
+  <si>
+    <t>/ccu-filing-doc:CourtCaseFilingDocument/cfd-ext:CourtCaseFilingAttachment/xop:Include/@href</t>
+  </si>
+  <si>
+    <t>/ccu-filing-doc:CourtCaseFilingDocument/nc:DocumentTitleText</t>
+  </si>
+  <si>
+    <t>/ccu-filing-doc:CourtCaseFilingDocument/j:Arrest/j:ArrestAgencyRecordIdentification/nc:IdentificationID</t>
+  </si>
+  <si>
+    <t>/ccu-filing-doc:CourtCaseFilingDocument/nc:Case/nc:CaseDocketID</t>
+  </si>
+  <si>
+    <t>/ccu-filing-doc:CourtCaseFilingDocument/nc:DocumentKeywordText</t>
+  </si>
+  <si>
+    <t>/ccu-filing-doc:CourtCaseFilingDocument/nc:DocumentDescriptionText</t>
+  </si>
+  <si>
+    <t>/ccu-filing-doc:CourtCaseFilingDocument/nc:DocumentAuthor/nc:EntityPerson</t>
+  </si>
+  <si>
+    <t>/ccu-filing-doc:CourtCaseFilingDocument/nc:PublisherName/nc:EntityPerson</t>
+  </si>
+  <si>
+    <t>/ccu-filing-doc:CourtCaseFilingDocument/nc:DocumentMediaCategoryText</t>
+  </si>
+  <si>
+    <t>/ccu-filing-doc:CourtCaseFilingDocument/nc:DocumentFormatText</t>
+  </si>
+  <si>
+    <t>/ccu-filing-doc:CourtCaseFilingDocument/nc:DocumentLanguageCode</t>
+  </si>
+  <si>
+    <t>/ccu-filing-doc:CourtCaseFilingDocument/nc:Person/nc:PersonDigitizedSignatureImage/nc:Base64BinaryObject</t>
   </si>
 </sst>
 </file>
@@ -1192,7 +1342,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1277,8 +1427,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1296,19 +1452,6 @@
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -1407,7 +1550,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1496,9 +1639,6 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="24" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="24" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1511,11 +1651,41 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="24" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="24" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="90">
@@ -1612,6 +1782,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1902,22 +2077,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I108"/>
+  <dimension ref="A1:I117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B95" sqref="B95:B98"/>
+    <sheetView topLeftCell="A97" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C100" sqref="C100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23" style="1" customWidth="1"/>
-    <col min="3" max="4" width="57.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="37" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="29.7109375" style="44" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23" style="34" customWidth="1"/>
+    <col min="3" max="4" width="57.28515625" style="34" customWidth="1"/>
+    <col min="5" max="5" width="37" style="34" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>82</v>
       </c>
@@ -1934,7 +2109,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>20</v>
       </c>
@@ -1943,7 +2118,7 @@
       <c r="D2" s="18"/>
       <c r="E2" s="18"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>11</v>
       </c>
@@ -1954,7 +2129,7 @@
       <c r="D3" s="28"/>
       <c r="E3" s="19"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>10</v>
       </c>
@@ -1965,7 +2140,7 @@
       <c r="D4" s="19"/>
       <c r="E4" s="19"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>12</v>
       </c>
@@ -1976,7 +2151,7 @@
       <c r="D5" s="23"/>
       <c r="E5" s="19"/>
     </row>
-    <row r="6" spans="1:5" ht="28">
+    <row r="6" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
         <v>13</v>
       </c>
@@ -1987,7 +2162,7 @@
       <c r="D6" s="19"/>
       <c r="E6" s="19"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
         <v>152</v>
       </c>
@@ -1998,7 +2173,7 @@
       <c r="D7" s="19"/>
       <c r="E7" s="19"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>4</v>
       </c>
@@ -2007,7 +2182,7 @@
       <c r="D8" s="18"/>
       <c r="E8" s="18"/>
     </row>
-    <row r="9" spans="1:5" ht="28">
+    <row r="9" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
         <v>32</v>
       </c>
@@ -2022,7 +2197,7 @@
       </c>
       <c r="E9" s="19"/>
     </row>
-    <row r="10" spans="1:5" ht="42">
+    <row r="10" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
         <v>33</v>
       </c>
@@ -2037,7 +2212,7 @@
       </c>
       <c r="E10" s="19"/>
     </row>
-    <row r="11" spans="1:5" ht="42">
+    <row r="11" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
         <v>34</v>
       </c>
@@ -2048,7 +2223,7 @@
       <c r="D11" s="23"/>
       <c r="E11" s="19"/>
     </row>
-    <row r="12" spans="1:5" ht="42">
+    <row r="12" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
         <v>35</v>
       </c>
@@ -2063,7 +2238,7 @@
       </c>
       <c r="E12" s="19"/>
     </row>
-    <row r="13" spans="1:5" ht="42">
+    <row r="13" spans="1:5" ht="51" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
         <v>36</v>
       </c>
@@ -2074,7 +2249,7 @@
       <c r="D13" s="19"/>
       <c r="E13" s="19"/>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>37</v>
       </c>
@@ -2084,7 +2259,7 @@
       </c>
       <c r="D14" s="19"/>
     </row>
-    <row r="15" spans="1:5" s="2" customFormat="1" ht="42">
+    <row r="15" spans="1:5" s="35" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A15" s="24" t="s">
         <v>0</v>
       </c>
@@ -2099,7 +2274,7 @@
       </c>
       <c r="E15" s="22"/>
     </row>
-    <row r="16" spans="1:5" s="2" customFormat="1" ht="42">
+    <row r="16" spans="1:5" s="35" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A16" s="24" t="s">
         <v>253</v>
       </c>
@@ -2112,7 +2287,7 @@
       </c>
       <c r="E16" s="26"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>222</v>
       </c>
@@ -2121,11 +2296,11 @@
       <c r="D17" s="18"/>
       <c r="E17" s="18"/>
     </row>
-    <row r="18" spans="1:5" s="2" customFormat="1" ht="28">
+    <row r="18" spans="1:5" s="35" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A18" s="24" t="s">
         <v>254</v>
       </c>
-      <c r="B18" s="33">
+      <c r="B18" s="32">
         <v>42257</v>
       </c>
       <c r="C18" s="26" t="s">
@@ -2136,7 +2311,7 @@
       </c>
       <c r="E18" s="26"/>
     </row>
-    <row r="19" spans="1:5" s="2" customFormat="1" ht="28">
+    <row r="19" spans="1:5" s="35" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A19" s="24" t="s">
         <v>255</v>
       </c>
@@ -2147,7 +2322,7 @@
       </c>
       <c r="E19" s="26"/>
     </row>
-    <row r="20" spans="1:5" s="2" customFormat="1" ht="42">
+    <row r="20" spans="1:5" s="35" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A20" s="24" t="s">
         <v>244</v>
       </c>
@@ -2158,7 +2333,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="2" customFormat="1" ht="42">
+    <row r="21" spans="1:5" s="35" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A21" s="24" t="s">
         <v>245</v>
       </c>
@@ -2171,7 +2346,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="22" spans="1:5" s="2" customFormat="1" ht="42">
+    <row r="22" spans="1:5" s="35" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A22" s="24" t="s">
         <v>248</v>
       </c>
@@ -2184,7 +2359,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
         <v>21</v>
       </c>
@@ -2193,7 +2368,7 @@
       <c r="D23" s="18"/>
       <c r="E23" s="18"/>
     </row>
-    <row r="24" spans="1:5" s="2" customFormat="1" ht="28">
+    <row r="24" spans="1:5" s="35" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A24" s="24" t="s">
         <v>3</v>
       </c>
@@ -2203,14 +2378,14 @@
       <c r="C24" s="26" t="s">
         <v>160</v>
       </c>
-      <c r="D24" s="30" t="s">
+      <c r="D24" s="36" t="s">
         <v>267</v>
       </c>
       <c r="E24" s="25" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="2" customFormat="1">
+    <row r="25" spans="1:5" s="35" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A25" s="24" t="s">
         <v>148</v>
       </c>
@@ -2225,11 +2400,11 @@
       </c>
       <c r="E25" s="26"/>
     </row>
-    <row r="26" spans="1:5" s="2" customFormat="1" ht="42">
+    <row r="26" spans="1:5" s="35" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A26" s="24" t="s">
         <v>149</v>
       </c>
-      <c r="B26" s="33">
+      <c r="B26" s="32">
         <v>42344</v>
       </c>
       <c r="C26" s="26" t="s">
@@ -2240,7 +2415,7 @@
       </c>
       <c r="E26" s="26"/>
     </row>
-    <row r="27" spans="1:5" s="2" customFormat="1" ht="28">
+    <row r="27" spans="1:5" s="35" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A27" s="24" t="s">
         <v>150</v>
       </c>
@@ -2250,18 +2425,18 @@
       <c r="C27" s="26" t="s">
         <v>162</v>
       </c>
-      <c r="D27" s="36" t="s">
+      <c r="D27" s="30" t="s">
         <v>284</v>
       </c>
       <c r="E27" s="25" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="28" spans="1:5" s="2" customFormat="1" ht="42">
+    <row r="28" spans="1:5" s="35" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A28" s="24" t="s">
         <v>151</v>
       </c>
-      <c r="B28" s="33">
+      <c r="B28" s="32">
         <v>42318</v>
       </c>
       <c r="C28" s="26" t="s">
@@ -2274,7 +2449,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="29" spans="1:5" s="2" customFormat="1" ht="42">
+    <row r="29" spans="1:5" s="35" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A29" s="24" t="s">
         <v>27</v>
       </c>
@@ -2289,7 +2464,7 @@
       </c>
       <c r="E29" s="26"/>
     </row>
-    <row r="30" spans="1:5" s="2" customFormat="1" ht="42">
+    <row r="30" spans="1:5" s="35" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A30" s="24" t="s">
         <v>26</v>
       </c>
@@ -2304,7 +2479,7 @@
       </c>
       <c r="E30" s="26"/>
     </row>
-    <row r="31" spans="1:5" s="2" customFormat="1" ht="42">
+    <row r="31" spans="1:5" s="35" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A31" s="24" t="s">
         <v>28</v>
       </c>
@@ -2321,7 +2496,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="32" spans="1:5" s="2" customFormat="1" ht="56">
+    <row r="32" spans="1:5" s="35" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A32" s="24" t="s">
         <v>29</v>
       </c>
@@ -2329,12 +2504,12 @@
       <c r="C32" s="26" t="s">
         <v>204</v>
       </c>
-      <c r="D32" s="31" t="s">
+      <c r="D32" s="30" t="s">
         <v>328</v>
       </c>
       <c r="E32" s="26"/>
     </row>
-    <row r="33" spans="1:5" s="2" customFormat="1" ht="42">
+    <row r="33" spans="1:5" s="35" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A33" s="24" t="s">
         <v>30</v>
       </c>
@@ -2345,7 +2520,7 @@
       <c r="D33" s="27"/>
       <c r="E33" s="26"/>
     </row>
-    <row r="34" spans="1:5" s="2" customFormat="1" ht="56">
+    <row r="34" spans="1:5" s="35" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A34" s="24" t="s">
         <v>31</v>
       </c>
@@ -2356,7 +2531,7 @@
       <c r="D34" s="26"/>
       <c r="E34" s="26"/>
     </row>
-    <row r="35" spans="1:5" s="2" customFormat="1" ht="42">
+    <row r="35" spans="1:5" s="35" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A35" s="24" t="s">
         <v>68</v>
       </c>
@@ -2367,7 +2542,7 @@
       <c r="D35" s="26"/>
       <c r="E35" s="26"/>
     </row>
-    <row r="36" spans="1:5" s="2" customFormat="1" ht="42">
+    <row r="36" spans="1:5" s="35" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A36" s="24" t="s">
         <v>65</v>
       </c>
@@ -2378,7 +2553,7 @@
       <c r="D36" s="26"/>
       <c r="E36" s="26"/>
     </row>
-    <row r="37" spans="1:5" s="2" customFormat="1" ht="56">
+    <row r="37" spans="1:5" s="35" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A37" s="24" t="s">
         <v>66</v>
       </c>
@@ -2389,7 +2564,7 @@
       <c r="D37" s="26"/>
       <c r="E37" s="26"/>
     </row>
-    <row r="38" spans="1:5" s="2" customFormat="1" ht="42">
+    <row r="38" spans="1:5" s="35" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A38" s="24" t="s">
         <v>67</v>
       </c>
@@ -2400,7 +2575,7 @@
       <c r="D38" s="26"/>
       <c r="E38" s="26"/>
     </row>
-    <row r="39" spans="1:5" s="2" customFormat="1" ht="56">
+    <row r="39" spans="1:5" s="35" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A39" s="24" t="s">
         <v>69</v>
       </c>
@@ -2415,7 +2590,7 @@
       </c>
       <c r="E39" s="29"/>
     </row>
-    <row r="40" spans="1:5" s="2" customFormat="1" ht="56">
+    <row r="40" spans="1:5" s="35" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A40" s="24" t="s">
         <v>70</v>
       </c>
@@ -2430,7 +2605,7 @@
       </c>
       <c r="E40" s="26"/>
     </row>
-    <row r="41" spans="1:5" s="2" customFormat="1" ht="56">
+    <row r="41" spans="1:5" s="35" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A41" s="24" t="s">
         <v>71</v>
       </c>
@@ -2441,7 +2616,7 @@
       <c r="D41" s="26"/>
       <c r="E41" s="26"/>
     </row>
-    <row r="42" spans="1:5" s="2" customFormat="1" ht="42">
+    <row r="42" spans="1:5" s="35" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A42" s="24" t="s">
         <v>72</v>
       </c>
@@ -2452,7 +2627,7 @@
       <c r="D42" s="26"/>
       <c r="E42" s="26"/>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="20" t="s">
         <v>5</v>
       </c>
@@ -2461,7 +2636,7 @@
       <c r="D43" s="18"/>
       <c r="E43" s="18"/>
     </row>
-    <row r="44" spans="1:5" s="2" customFormat="1" ht="42">
+    <row r="44" spans="1:5" s="35" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A44" s="24" t="s">
         <v>14</v>
       </c>
@@ -2472,7 +2647,7 @@
       <c r="D44" s="26"/>
       <c r="E44" s="26"/>
     </row>
-    <row r="45" spans="1:5" s="2" customFormat="1" ht="42">
+    <row r="45" spans="1:5" s="35" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A45" s="24" t="s">
         <v>15</v>
       </c>
@@ -2483,7 +2658,7 @@
       <c r="D45" s="26"/>
       <c r="E45" s="26"/>
     </row>
-    <row r="46" spans="1:5" s="2" customFormat="1" ht="42">
+    <row r="46" spans="1:5" s="35" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A46" s="24" t="s">
         <v>16</v>
       </c>
@@ -2498,7 +2673,7 @@
       </c>
       <c r="E46" s="26"/>
     </row>
-    <row r="47" spans="1:5" s="2" customFormat="1" ht="42">
+    <row r="47" spans="1:5" s="35" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A47" s="24" t="s">
         <v>17</v>
       </c>
@@ -2513,7 +2688,7 @@
       </c>
       <c r="E47" s="26"/>
     </row>
-    <row r="48" spans="1:5" s="2" customFormat="1" ht="42">
+    <row r="48" spans="1:5" s="35" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A48" s="24" t="s">
         <v>18</v>
       </c>
@@ -2530,7 +2705,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="49" spans="1:5" s="2" customFormat="1" ht="28">
+    <row r="49" spans="1:5" s="35" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A49" s="25" t="s">
         <v>258</v>
       </c>
@@ -2538,14 +2713,14 @@
         <v>301</v>
       </c>
       <c r="C49" s="26"/>
-      <c r="D49" s="32" t="s">
+      <c r="D49" s="31" t="s">
         <v>243</v>
       </c>
       <c r="E49" s="26" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="50" spans="1:5" s="2" customFormat="1" ht="42">
+    <row r="50" spans="1:5" s="35" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A50" s="24" t="s">
         <v>22</v>
       </c>
@@ -2560,7 +2735,7 @@
       </c>
       <c r="E50" s="26"/>
     </row>
-    <row r="51" spans="1:5" s="2" customFormat="1" ht="56">
+    <row r="51" spans="1:5" s="35" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A51" s="24" t="s">
         <v>19</v>
       </c>
@@ -2571,7 +2746,7 @@
       <c r="D51" s="28"/>
       <c r="E51" s="26"/>
     </row>
-    <row r="52" spans="1:5" s="2" customFormat="1" ht="42">
+    <row r="52" spans="1:5" s="35" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A52" s="24" t="s">
         <v>23</v>
       </c>
@@ -2586,7 +2761,7 @@
       </c>
       <c r="E52" s="26"/>
     </row>
-    <row r="53" spans="1:5" s="2" customFormat="1" ht="42">
+    <row r="53" spans="1:5" s="35" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A53" s="24" t="s">
         <v>24</v>
       </c>
@@ -2601,7 +2776,7 @@
       </c>
       <c r="E53" s="26"/>
     </row>
-    <row r="54" spans="1:5" s="2" customFormat="1" ht="42">
+    <row r="54" spans="1:5" s="35" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A54" s="24" t="s">
         <v>25</v>
       </c>
@@ -2612,7 +2787,7 @@
       <c r="D54" s="26"/>
       <c r="E54" s="26"/>
     </row>
-    <row r="55" spans="1:5" s="2" customFormat="1" ht="42">
+    <row r="55" spans="1:5" s="35" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A55" s="24" t="s">
         <v>197</v>
       </c>
@@ -2623,7 +2798,7 @@
       <c r="D55" s="26"/>
       <c r="E55" s="25"/>
     </row>
-    <row r="56" spans="1:5" s="2" customFormat="1" ht="38" customHeight="1">
+    <row r="56" spans="1:5" s="35" customFormat="1" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="24" t="s">
         <v>242</v>
       </c>
@@ -2632,7 +2807,7 @@
       <c r="D56" s="25"/>
       <c r="E56" s="25"/>
     </row>
-    <row r="57" spans="1:5" s="2" customFormat="1" ht="42">
+    <row r="57" spans="1:5" s="35" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A57" s="24" t="s">
         <v>145</v>
       </c>
@@ -2643,7 +2818,7 @@
       <c r="D57" s="25"/>
       <c r="E57" s="28"/>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="20" t="s">
         <v>6</v>
       </c>
@@ -2652,7 +2827,7 @@
       <c r="D58" s="18"/>
       <c r="E58" s="18"/>
     </row>
-    <row r="59" spans="1:5" s="2" customFormat="1" ht="28">
+    <row r="59" spans="1:5" s="35" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A59" s="24" t="s">
         <v>38</v>
       </c>
@@ -2667,7 +2842,7 @@
       </c>
       <c r="E59" s="26"/>
     </row>
-    <row r="60" spans="1:5" s="2" customFormat="1" ht="28">
+    <row r="60" spans="1:5" s="35" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A60" s="24" t="s">
         <v>39</v>
       </c>
@@ -2682,7 +2857,7 @@
       </c>
       <c r="E60" s="26"/>
     </row>
-    <row r="61" spans="1:5" s="2" customFormat="1" ht="28">
+    <row r="61" spans="1:5" s="35" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A61" s="24" t="s">
         <v>40</v>
       </c>
@@ -2697,7 +2872,7 @@
       </c>
       <c r="E61" s="26"/>
     </row>
-    <row r="62" spans="1:5" s="2" customFormat="1" ht="42">
+    <row r="62" spans="1:5" s="35" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A62" s="24" t="s">
         <v>41</v>
       </c>
@@ -2712,7 +2887,7 @@
       </c>
       <c r="E62" s="26"/>
     </row>
-    <row r="63" spans="1:5" s="2" customFormat="1" ht="28">
+    <row r="63" spans="1:5" s="35" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A63" s="24" t="s">
         <v>42</v>
       </c>
@@ -2727,11 +2902,11 @@
       </c>
       <c r="E63" s="26"/>
     </row>
-    <row r="64" spans="1:5" s="2" customFormat="1" ht="28">
+    <row r="64" spans="1:5" s="35" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A64" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="B64" s="33">
+      <c r="B64" s="32">
         <v>29521</v>
       </c>
       <c r="C64" s="26" t="s">
@@ -2742,7 +2917,7 @@
       </c>
       <c r="E64" s="26"/>
     </row>
-    <row r="65" spans="1:5" s="2" customFormat="1" ht="42">
+    <row r="65" spans="1:5" s="35" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A65" s="24" t="s">
         <v>45</v>
       </c>
@@ -2757,7 +2932,7 @@
       </c>
       <c r="E65" s="26"/>
     </row>
-    <row r="66" spans="1:5" s="2" customFormat="1" ht="42">
+    <row r="66" spans="1:5" s="35" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A66" s="24" t="s">
         <v>259</v>
       </c>
@@ -2770,7 +2945,7 @@
       </c>
       <c r="E66" s="26"/>
     </row>
-    <row r="67" spans="1:5" s="2" customFormat="1" ht="42">
+    <row r="67" spans="1:5" s="35" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A67" s="24" t="s">
         <v>48</v>
       </c>
@@ -2781,7 +2956,7 @@
       <c r="D67" s="24"/>
       <c r="E67" s="26"/>
     </row>
-    <row r="68" spans="1:5" s="2" customFormat="1" ht="42">
+    <row r="68" spans="1:5" s="35" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A68" s="24" t="s">
         <v>46</v>
       </c>
@@ -2796,7 +2971,7 @@
       </c>
       <c r="E68" s="26"/>
     </row>
-    <row r="69" spans="1:5" s="2" customFormat="1" ht="28">
+    <row r="69" spans="1:5" s="35" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A69" s="24" t="s">
         <v>260</v>
       </c>
@@ -2804,12 +2979,12 @@
         <v>46</v>
       </c>
       <c r="C69" s="26"/>
-      <c r="D69" s="34" t="s">
+      <c r="D69" s="33" t="s">
         <v>224</v>
       </c>
       <c r="E69" s="26"/>
     </row>
-    <row r="70" spans="1:5" s="2" customFormat="1" ht="42">
+    <row r="70" spans="1:5" s="35" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A70" s="24" t="s">
         <v>47</v>
       </c>
@@ -2817,10 +2992,10 @@
       <c r="C70" s="26" t="s">
         <v>193</v>
       </c>
-      <c r="D70" s="35"/>
+      <c r="D70" s="33"/>
       <c r="E70" s="26"/>
     </row>
-    <row r="71" spans="1:5" s="2" customFormat="1" ht="42">
+    <row r="71" spans="1:5" s="35" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A71" s="24" t="s">
         <v>49</v>
       </c>
@@ -2835,7 +3010,7 @@
       </c>
       <c r="E71" s="26"/>
     </row>
-    <row r="72" spans="1:5" s="2" customFormat="1" ht="42">
+    <row r="72" spans="1:5" s="35" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A72" s="24" t="s">
         <v>228</v>
       </c>
@@ -2848,7 +3023,7 @@
       </c>
       <c r="E72" s="26"/>
     </row>
-    <row r="73" spans="1:5" s="2" customFormat="1" ht="42">
+    <row r="73" spans="1:5" s="35" customFormat="1" ht="51" x14ac:dyDescent="0.25">
       <c r="A73" s="24" t="s">
         <v>50</v>
       </c>
@@ -2863,7 +3038,7 @@
       </c>
       <c r="E73" s="26"/>
     </row>
-    <row r="74" spans="1:5" s="2" customFormat="1" ht="28">
+    <row r="74" spans="1:5" s="35" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A74" s="24" t="s">
         <v>226</v>
       </c>
@@ -2878,7 +3053,7 @@
       </c>
       <c r="E74" s="26"/>
     </row>
-    <row r="75" spans="1:5" s="2" customFormat="1" ht="42">
+    <row r="75" spans="1:5" s="35" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A75" s="24" t="s">
         <v>227</v>
       </c>
@@ -2891,7 +3066,7 @@
       </c>
       <c r="E75" s="26"/>
     </row>
-    <row r="76" spans="1:5" s="2" customFormat="1" ht="28">
+    <row r="76" spans="1:5" s="35" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A76" s="24" t="s">
         <v>146</v>
       </c>
@@ -2906,7 +3081,7 @@
       </c>
       <c r="E76" s="26"/>
     </row>
-    <row r="77" spans="1:5" s="2" customFormat="1" ht="42">
+    <row r="77" spans="1:5" s="35" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A77" s="24" t="s">
         <v>147</v>
       </c>
@@ -2921,7 +3096,7 @@
       </c>
       <c r="E77" s="26"/>
     </row>
-    <row r="78" spans="1:5" s="2" customFormat="1" ht="42">
+    <row r="78" spans="1:5" s="35" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A78" s="24" t="s">
         <v>153</v>
       </c>
@@ -2932,7 +3107,7 @@
       <c r="D78" s="26"/>
       <c r="E78" s="26"/>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="20" t="s">
         <v>234</v>
       </c>
@@ -2943,7 +3118,7 @@
       <c r="D79" s="18"/>
       <c r="E79" s="18"/>
     </row>
-    <row r="80" spans="1:5" ht="42">
+    <row r="80" spans="1:5" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A80" s="21" t="s">
         <v>73</v>
       </c>
@@ -2954,7 +3129,7 @@
       <c r="D80" s="19"/>
       <c r="E80" s="19"/>
     </row>
-    <row r="81" spans="1:9" ht="28">
+    <row r="81" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A81" s="24" t="s">
         <v>52</v>
       </c>
@@ -2965,7 +3140,7 @@
       <c r="D81" s="19"/>
       <c r="E81" s="19"/>
     </row>
-    <row r="82" spans="1:9" ht="28">
+    <row r="82" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A82" s="24" t="s">
         <v>53</v>
       </c>
@@ -2975,12 +3150,12 @@
       </c>
       <c r="D82" s="19"/>
       <c r="E82" s="19"/>
-      <c r="F82" s="3"/>
-      <c r="G82" s="3"/>
-      <c r="H82" s="3"/>
-      <c r="I82" s="3"/>
-    </row>
-    <row r="83" spans="1:9" ht="28">
+      <c r="F82" s="37"/>
+      <c r="G82" s="37"/>
+      <c r="H82" s="37"/>
+      <c r="I82" s="37"/>
+    </row>
+    <row r="83" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A83" s="24" t="s">
         <v>54</v>
       </c>
@@ -2990,12 +3165,12 @@
       </c>
       <c r="D83" s="19"/>
       <c r="E83" s="19"/>
-      <c r="F83" s="3"/>
-      <c r="G83" s="3"/>
-      <c r="H83" s="3"/>
-      <c r="I83" s="3"/>
-    </row>
-    <row r="84" spans="1:9" ht="42">
+      <c r="F83" s="37"/>
+      <c r="G83" s="37"/>
+      <c r="H83" s="37"/>
+      <c r="I83" s="37"/>
+    </row>
+    <row r="84" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A84" s="24" t="s">
         <v>55</v>
       </c>
@@ -3005,12 +3180,12 @@
       </c>
       <c r="D84" s="19"/>
       <c r="E84" s="19"/>
-      <c r="F84" s="3"/>
-      <c r="G84" s="3"/>
-      <c r="H84" s="3"/>
-      <c r="I84" s="3"/>
-    </row>
-    <row r="85" spans="1:9" ht="28">
+      <c r="F84" s="37"/>
+      <c r="G84" s="37"/>
+      <c r="H84" s="37"/>
+      <c r="I84" s="37"/>
+    </row>
+    <row r="85" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A85" s="24" t="s">
         <v>56</v>
       </c>
@@ -3024,12 +3199,12 @@
         <v>236</v>
       </c>
       <c r="E85" s="19"/>
-      <c r="F85" s="3"/>
-      <c r="G85" s="3"/>
-      <c r="H85" s="3"/>
-      <c r="I85" s="3"/>
-    </row>
-    <row r="86" spans="1:9">
+      <c r="F85" s="37"/>
+      <c r="G85" s="37"/>
+      <c r="H85" s="37"/>
+      <c r="I85" s="37"/>
+    </row>
+    <row r="86" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A86" s="20" t="s">
         <v>31</v>
       </c>
@@ -3039,12 +3214,12 @@
       </c>
       <c r="D86" s="18"/>
       <c r="E86" s="18"/>
-      <c r="F86" s="3"/>
-      <c r="G86" s="3"/>
-      <c r="H86" s="3"/>
-      <c r="I86" s="3"/>
-    </row>
-    <row r="87" spans="1:9" ht="42">
+      <c r="F86" s="37"/>
+      <c r="G86" s="37"/>
+      <c r="H86" s="37"/>
+      <c r="I86" s="37"/>
+    </row>
+    <row r="87" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A87" s="21" t="s">
         <v>57</v>
       </c>
@@ -3054,12 +3229,12 @@
       </c>
       <c r="D87" s="19"/>
       <c r="E87" s="19"/>
-      <c r="F87" s="3"/>
-      <c r="G87" s="3"/>
-      <c r="H87" s="3"/>
-      <c r="I87" s="3"/>
-    </row>
-    <row r="88" spans="1:9" ht="42">
+      <c r="F87" s="37"/>
+      <c r="G87" s="37"/>
+      <c r="H87" s="37"/>
+      <c r="I87" s="37"/>
+    </row>
+    <row r="88" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A88" s="21" t="s">
         <v>58</v>
       </c>
@@ -3069,12 +3244,12 @@
       </c>
       <c r="D88" s="19"/>
       <c r="E88" s="19"/>
-      <c r="F88" s="3"/>
-      <c r="G88" s="3"/>
-      <c r="H88" s="3"/>
-      <c r="I88" s="3"/>
-    </row>
-    <row r="89" spans="1:9" ht="42">
+      <c r="F88" s="37"/>
+      <c r="G88" s="37"/>
+      <c r="H88" s="37"/>
+      <c r="I88" s="37"/>
+    </row>
+    <row r="89" spans="1:9" ht="51" x14ac:dyDescent="0.25">
       <c r="A89" s="21" t="s">
         <v>59</v>
       </c>
@@ -3084,12 +3259,12 @@
       </c>
       <c r="D89" s="19"/>
       <c r="E89" s="19"/>
-      <c r="F89" s="3"/>
-      <c r="G89" s="3"/>
-      <c r="H89" s="3"/>
-      <c r="I89" s="3"/>
-    </row>
-    <row r="90" spans="1:9" ht="28">
+      <c r="F89" s="37"/>
+      <c r="G89" s="37"/>
+      <c r="H89" s="37"/>
+      <c r="I89" s="37"/>
+    </row>
+    <row r="90" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A90" s="21" t="s">
         <v>60</v>
       </c>
@@ -3099,12 +3274,12 @@
       </c>
       <c r="D90" s="19"/>
       <c r="E90" s="19"/>
-      <c r="F90" s="3"/>
-      <c r="G90" s="3"/>
-      <c r="H90" s="3"/>
-      <c r="I90" s="3"/>
-    </row>
-    <row r="91" spans="1:9">
+      <c r="F90" s="37"/>
+      <c r="G90" s="37"/>
+      <c r="H90" s="37"/>
+      <c r="I90" s="37"/>
+    </row>
+    <row r="91" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A91" s="20" t="s">
         <v>235</v>
       </c>
@@ -3114,12 +3289,12 @@
       </c>
       <c r="D91" s="18"/>
       <c r="E91" s="18"/>
-      <c r="F91" s="3"/>
-      <c r="G91" s="3"/>
-      <c r="H91" s="3"/>
-      <c r="I91" s="3"/>
-    </row>
-    <row r="92" spans="1:9" ht="28">
+      <c r="F91" s="37"/>
+      <c r="G91" s="37"/>
+      <c r="H91" s="37"/>
+      <c r="I91" s="37"/>
+    </row>
+    <row r="92" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A92" s="21" t="s">
         <v>209</v>
       </c>
@@ -3133,12 +3308,12 @@
         <v>237</v>
       </c>
       <c r="E92" s="19"/>
-      <c r="F92" s="3"/>
-      <c r="G92" s="3"/>
-      <c r="H92" s="3"/>
-      <c r="I92" s="3"/>
-    </row>
-    <row r="93" spans="1:9">
+      <c r="F92" s="37"/>
+      <c r="G92" s="37"/>
+      <c r="H92" s="37"/>
+      <c r="I92" s="37"/>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="20" t="s">
         <v>231</v>
       </c>
@@ -3148,12 +3323,12 @@
       </c>
       <c r="D93" s="18"/>
       <c r="E93" s="18"/>
-      <c r="F93" s="3"/>
-      <c r="G93" s="3"/>
-      <c r="H93" s="3"/>
-      <c r="I93" s="3"/>
-    </row>
-    <row r="94" spans="1:9">
+      <c r="F93" s="37"/>
+      <c r="G93" s="37"/>
+      <c r="H93" s="37"/>
+      <c r="I93" s="37"/>
+    </row>
+    <row r="94" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A94" s="21" t="s">
         <v>211</v>
       </c>
@@ -3163,12 +3338,12 @@
       </c>
       <c r="D94" s="19"/>
       <c r="E94" s="19"/>
-      <c r="F94" s="3"/>
-      <c r="G94" s="3"/>
-      <c r="H94" s="3"/>
-      <c r="I94" s="3"/>
-    </row>
-    <row r="95" spans="1:9" ht="56">
+      <c r="F94" s="37"/>
+      <c r="G94" s="37"/>
+      <c r="H94" s="37"/>
+      <c r="I94" s="37"/>
+    </row>
+    <row r="95" spans="1:9" ht="51" x14ac:dyDescent="0.25">
       <c r="A95" s="21" t="s">
         <v>212</v>
       </c>
@@ -3182,12 +3357,12 @@
         <v>230</v>
       </c>
       <c r="E95" s="19"/>
-      <c r="F95" s="3"/>
-      <c r="G95" s="3"/>
-      <c r="H95" s="3"/>
-      <c r="I95" s="3"/>
-    </row>
-    <row r="96" spans="1:9" ht="42">
+      <c r="F95" s="37"/>
+      <c r="G95" s="37"/>
+      <c r="H95" s="37"/>
+      <c r="I95" s="37"/>
+    </row>
+    <row r="96" spans="1:9" ht="51" x14ac:dyDescent="0.25">
       <c r="A96" s="21" t="s">
         <v>213</v>
       </c>
@@ -3201,12 +3376,12 @@
         <v>232</v>
       </c>
       <c r="E96" s="19"/>
-      <c r="F96" s="3"/>
-      <c r="G96" s="3"/>
-      <c r="H96" s="3"/>
-      <c r="I96" s="3"/>
-    </row>
-    <row r="97" spans="1:9" ht="42">
+      <c r="F96" s="37"/>
+      <c r="G96" s="37"/>
+      <c r="H96" s="37"/>
+      <c r="I96" s="37"/>
+    </row>
+    <row r="97" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A97" s="21" t="s">
         <v>214</v>
       </c>
@@ -3216,12 +3391,12 @@
       </c>
       <c r="D97" s="19"/>
       <c r="E97" s="19"/>
-      <c r="F97" s="3"/>
-      <c r="G97" s="3"/>
-      <c r="H97" s="3"/>
-      <c r="I97" s="3"/>
-    </row>
-    <row r="98" spans="1:9" ht="42">
+      <c r="F97" s="37"/>
+      <c r="G97" s="37"/>
+      <c r="H97" s="37"/>
+      <c r="I97" s="37"/>
+    </row>
+    <row r="98" spans="1:9" ht="51" x14ac:dyDescent="0.25">
       <c r="A98" s="21" t="s">
         <v>215</v>
       </c>
@@ -3235,124 +3410,279 @@
         <v>233</v>
       </c>
       <c r="E98" s="19"/>
-      <c r="F98" s="3"/>
-      <c r="G98" s="3"/>
-      <c r="H98" s="3"/>
-      <c r="I98" s="3"/>
-    </row>
-    <row r="99" spans="1:9">
-      <c r="A99" s="10"/>
-      <c r="B99" s="3"/>
-      <c r="C99" s="3"/>
-      <c r="D99" s="3"/>
-      <c r="E99" s="3"/>
-      <c r="F99" s="3"/>
-      <c r="G99" s="3"/>
-      <c r="H99" s="3"/>
-      <c r="I99" s="3"/>
-    </row>
-    <row r="100" spans="1:9">
-      <c r="A100" s="10"/>
-      <c r="B100" s="3"/>
-      <c r="C100" s="3"/>
-      <c r="D100" s="3"/>
-      <c r="E100" s="3"/>
-      <c r="F100" s="3"/>
-      <c r="G100" s="3"/>
-      <c r="H100" s="3"/>
-      <c r="I100" s="3"/>
-    </row>
-    <row r="101" spans="1:9">
-      <c r="A101" s="10"/>
-      <c r="B101" s="3"/>
-      <c r="C101" s="3"/>
-      <c r="D101" s="3"/>
-      <c r="E101" s="3"/>
-      <c r="F101" s="3"/>
-      <c r="G101" s="3"/>
-      <c r="H101" s="3"/>
-      <c r="I101" s="3"/>
-    </row>
-    <row r="102" spans="1:9">
-      <c r="A102" s="10"/>
-      <c r="B102" s="3"/>
-      <c r="C102" s="3"/>
-      <c r="D102" s="3"/>
-      <c r="E102" s="3"/>
-      <c r="F102" s="3"/>
-      <c r="G102" s="3"/>
-      <c r="H102" s="3"/>
-      <c r="I102" s="3"/>
-    </row>
-    <row r="103" spans="1:9">
-      <c r="A103" s="10"/>
-      <c r="B103" s="3"/>
-      <c r="C103" s="3"/>
-      <c r="D103" s="3"/>
-      <c r="E103" s="3"/>
-      <c r="F103" s="3"/>
-      <c r="G103" s="3"/>
-      <c r="H103" s="3"/>
-      <c r="I103" s="3"/>
-    </row>
-    <row r="104" spans="1:9">
-      <c r="A104" s="10"/>
-      <c r="B104" s="3"/>
-      <c r="C104" s="3"/>
-      <c r="D104" s="3"/>
-      <c r="E104" s="3"/>
-      <c r="F104" s="3"/>
-      <c r="G104" s="3"/>
-      <c r="H104" s="3"/>
-      <c r="I104" s="3"/>
-    </row>
-    <row r="105" spans="1:9">
-      <c r="A105" s="10"/>
-      <c r="B105" s="3"/>
-      <c r="C105" s="3"/>
-      <c r="D105" s="3"/>
-      <c r="E105" s="3"/>
-      <c r="F105" s="3"/>
-      <c r="G105" s="3"/>
-      <c r="H105" s="3"/>
-      <c r="I105" s="3"/>
-    </row>
-    <row r="106" spans="1:9">
-      <c r="A106" s="10"/>
-      <c r="B106" s="3"/>
-      <c r="C106" s="3"/>
-      <c r="D106" s="3"/>
-      <c r="E106" s="3"/>
-      <c r="F106" s="3"/>
-      <c r="G106" s="3"/>
-      <c r="H106" s="3"/>
-      <c r="I106" s="3"/>
-    </row>
-    <row r="107" spans="1:9">
-      <c r="A107" s="10"/>
-      <c r="B107" s="3"/>
-      <c r="C107" s="3"/>
-      <c r="D107" s="3"/>
-      <c r="E107" s="3"/>
-      <c r="F107" s="3"/>
-      <c r="G107" s="3"/>
-      <c r="H107" s="3"/>
-      <c r="I107" s="3"/>
-    </row>
-    <row r="108" spans="1:9">
-      <c r="A108" s="10"/>
-      <c r="B108" s="3"/>
-      <c r="C108" s="3"/>
-      <c r="D108" s="3"/>
-      <c r="E108" s="3"/>
-      <c r="F108" s="3"/>
-      <c r="G108" s="3"/>
-      <c r="H108" s="3"/>
-      <c r="I108" s="3"/>
+      <c r="F98" s="37"/>
+      <c r="G98" s="37"/>
+      <c r="H98" s="37"/>
+      <c r="I98" s="37"/>
+    </row>
+    <row r="99" spans="1:9" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="B99" s="38"/>
+      <c r="C99" s="39"/>
+      <c r="D99" s="39"/>
+      <c r="E99" s="39"/>
+      <c r="F99" s="40"/>
+      <c r="G99" s="40"/>
+      <c r="H99" s="40"/>
+      <c r="I99" s="40"/>
+    </row>
+    <row r="100" spans="1:9" ht="24" x14ac:dyDescent="0.25">
+      <c r="A100" s="42" t="s">
+        <v>331</v>
+      </c>
+      <c r="B100" s="37"/>
+      <c r="C100" s="37" t="s">
+        <v>358</v>
+      </c>
+      <c r="D100" s="37"/>
+      <c r="E100" s="37"/>
+      <c r="F100" s="37"/>
+      <c r="G100" s="37"/>
+      <c r="H100" s="37"/>
+      <c r="I100" s="37"/>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A101" s="42" t="s">
+        <v>332</v>
+      </c>
+      <c r="B101" s="37" t="s">
+        <v>333</v>
+      </c>
+      <c r="C101" s="37" t="s">
+        <v>359</v>
+      </c>
+      <c r="D101" s="37"/>
+      <c r="E101" s="37"/>
+      <c r="F101" s="37"/>
+      <c r="G101" s="37"/>
+      <c r="H101" s="37"/>
+      <c r="I101" s="37"/>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A102" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="B102" s="43">
+        <v>43101</v>
+      </c>
+      <c r="C102" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D102" s="37"/>
+      <c r="E102" s="37"/>
+      <c r="F102" s="37"/>
+      <c r="G102" s="37"/>
+      <c r="H102" s="37"/>
+      <c r="I102" s="37"/>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A103" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="B103" s="43">
+        <v>43115</v>
+      </c>
+      <c r="C103" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="D103" s="37"/>
+      <c r="E103" s="37"/>
+      <c r="F103" s="37"/>
+      <c r="G103" s="37"/>
+      <c r="H103" s="37"/>
+      <c r="I103" s="37"/>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A104" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="B104" s="43">
+        <v>43132</v>
+      </c>
+      <c r="C104" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="D104" s="37"/>
+      <c r="E104" s="37"/>
+      <c r="F104" s="37"/>
+      <c r="G104" s="37"/>
+      <c r="H104" s="37"/>
+      <c r="I104" s="37"/>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A105" s="42" t="s">
+        <v>334</v>
+      </c>
+      <c r="B105" s="37" t="s">
+        <v>335</v>
+      </c>
+      <c r="C105" s="37" t="s">
+        <v>360</v>
+      </c>
+      <c r="D105" s="37"/>
+      <c r="E105" s="37"/>
+      <c r="F105" s="37"/>
+      <c r="G105" s="37"/>
+      <c r="H105" s="37"/>
+      <c r="I105" s="37"/>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A106" s="42" t="s">
+        <v>336</v>
+      </c>
+      <c r="B106" s="37">
+        <v>330001234</v>
+      </c>
+      <c r="C106" s="37"/>
+      <c r="D106" s="37"/>
+      <c r="E106" s="37"/>
+      <c r="F106" s="37"/>
+      <c r="G106" s="37"/>
+      <c r="H106" s="37"/>
+      <c r="I106" s="37"/>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A107" s="42" t="s">
+        <v>337</v>
+      </c>
+      <c r="B107" s="37" t="s">
+        <v>338</v>
+      </c>
+      <c r="C107" s="37" t="s">
+        <v>156</v>
+      </c>
+      <c r="D107" s="37"/>
+      <c r="E107" s="37"/>
+      <c r="F107" s="37"/>
+      <c r="G107" s="37"/>
+      <c r="H107" s="37"/>
+      <c r="I107" s="37"/>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A108" s="42" t="s">
+        <v>339</v>
+      </c>
+      <c r="B108" s="37" t="s">
+        <v>340</v>
+      </c>
+      <c r="C108" s="37"/>
+      <c r="D108" s="37"/>
+      <c r="E108" s="37"/>
+      <c r="F108" s="37"/>
+      <c r="G108" s="37"/>
+      <c r="H108" s="37"/>
+      <c r="I108" s="37"/>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A109" s="42" t="s">
+        <v>341</v>
+      </c>
+      <c r="B109" s="37" t="s">
+        <v>342</v>
+      </c>
+      <c r="C109" s="37" t="s">
+        <v>160</v>
+      </c>
+      <c r="D109" s="37"/>
+      <c r="E109" s="37"/>
+      <c r="F109" s="37"/>
+      <c r="G109" s="37"/>
+      <c r="H109" s="37"/>
+      <c r="I109" s="37"/>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A110" s="44" t="s">
+        <v>343</v>
+      </c>
+      <c r="B110" s="34" t="s">
+        <v>344</v>
+      </c>
+      <c r="C110" s="34" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A111" s="44" t="s">
+        <v>345</v>
+      </c>
+      <c r="B111" s="34" t="s">
+        <v>346</v>
+      </c>
+      <c r="C111" s="34" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A112" s="44" t="s">
+        <v>347</v>
+      </c>
+      <c r="B112" s="34" t="s">
+        <v>348</v>
+      </c>
+      <c r="C112" s="34" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="44" t="s">
+        <v>349</v>
+      </c>
+      <c r="B113" s="34" t="s">
+        <v>350</v>
+      </c>
+      <c r="C113" s="34" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="44" t="s">
+        <v>351</v>
+      </c>
+      <c r="B114" s="34" t="s">
+        <v>352</v>
+      </c>
+      <c r="C114" s="34" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="44" t="s">
+        <v>353</v>
+      </c>
+      <c r="B115" s="34" t="s">
+        <v>354</v>
+      </c>
+      <c r="C115" s="34" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="44" t="s">
+        <v>355</v>
+      </c>
+      <c r="B116" s="34" t="s">
+        <v>356</v>
+      </c>
+      <c r="C116" s="34" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="44" t="s">
+        <v>44</v>
+      </c>
+      <c r="B117" s="34" t="s">
+        <v>357</v>
+      </c>
+      <c r="C117" s="34" t="s">
+        <v>368</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3363,21 +3693,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C83"/>
+  <dimension ref="A1:C88"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="A70" sqref="A70:C70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.83203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="152.6640625" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="32.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="152.7109375" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>82</v>
       </c>
@@ -3388,14 +3718,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>20</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="9"/>
     </row>
-    <row r="3" spans="1:3" ht="12" customHeight="1">
+    <row r="3" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>2</v>
       </c>
@@ -3404,7 +3734,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="12" customHeight="1">
+    <row r="4" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>11</v>
       </c>
@@ -3413,7 +3743,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="12" customHeight="1">
+    <row r="5" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>10</v>
       </c>
@@ -3422,7 +3752,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="12" customHeight="1">
+    <row r="6" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>12</v>
       </c>
@@ -3431,7 +3761,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="12" customHeight="1">
+    <row r="7" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>13</v>
       </c>
@@ -3440,14 +3770,14 @@
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="9"/>
     </row>
-    <row r="9" spans="1:3" ht="12" customHeight="1">
+    <row r="9" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>32</v>
       </c>
@@ -3456,7 +3786,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="12" customHeight="1">
+    <row r="10" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>33</v>
       </c>
@@ -3465,7 +3795,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="12" customHeight="1">
+    <row r="11" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>34</v>
       </c>
@@ -3474,7 +3804,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="12" customHeight="1">
+    <row r="12" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>35</v>
       </c>
@@ -3483,7 +3813,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="12" customHeight="1">
+    <row r="13" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>36</v>
       </c>
@@ -3492,7 +3822,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="12" customHeight="1">
+    <row r="14" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>37</v>
       </c>
@@ -3501,7 +3831,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="15" spans="1:3" s="2" customFormat="1" ht="12" customHeight="1">
+    <row r="15" spans="1:3" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>0</v>
       </c>
@@ -3510,14 +3840,14 @@
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>21</v>
       </c>
       <c r="B16" s="7"/>
       <c r="C16" s="9"/>
     </row>
-    <row r="17" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="17" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>3</v>
       </c>
@@ -3526,7 +3856,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="18" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>27</v>
       </c>
@@ -3535,7 +3865,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="19" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>26</v>
       </c>
@@ -3544,7 +3874,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="20" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>28</v>
       </c>
@@ -3553,7 +3883,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="21" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>29</v>
       </c>
@@ -3562,7 +3892,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="22" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>30</v>
       </c>
@@ -3571,7 +3901,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="23" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>31</v>
       </c>
@@ -3580,7 +3910,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="24" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
         <v>68</v>
       </c>
@@ -3589,7 +3919,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="25" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="25" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
         <v>65</v>
       </c>
@@ -3598,7 +3928,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="26" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="26" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>66</v>
       </c>
@@ -3607,7 +3937,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="27" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="27" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>67</v>
       </c>
@@ -3616,7 +3946,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="28" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="28" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>69</v>
       </c>
@@ -3625,7 +3955,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="29" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>70</v>
       </c>
@@ -3634,7 +3964,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="30" spans="1:3" s="2" customFormat="1" ht="12" customHeight="1">
+    <row r="30" spans="1:3" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>71</v>
       </c>
@@ -3643,7 +3973,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="31" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="31" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>72</v>
       </c>
@@ -3652,14 +3982,14 @@
         <v>109</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
         <v>5</v>
       </c>
       <c r="B32" s="7"/>
       <c r="C32" s="9"/>
     </row>
-    <row r="33" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="33" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
         <v>14</v>
       </c>
@@ -3668,7 +3998,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="34" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="34" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>15</v>
       </c>
@@ -3677,7 +4007,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="35" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="35" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
         <v>16</v>
       </c>
@@ -3686,7 +4016,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="36" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
         <v>17</v>
       </c>
@@ -3695,7 +4025,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="37" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="37" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
         <v>18</v>
       </c>
@@ -3704,7 +4034,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="38" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="38" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>22</v>
       </c>
@@ -3713,7 +4043,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="39" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="39" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
         <v>19</v>
       </c>
@@ -3722,7 +4052,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="40" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="40" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
         <v>23</v>
       </c>
@@ -3731,7 +4061,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="41" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="41" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
         <v>24</v>
       </c>
@@ -3740,7 +4070,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="42" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="42" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
         <v>25</v>
       </c>
@@ -3749,14 +4079,14 @@
         <v>119</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="14" t="s">
         <v>6</v>
       </c>
       <c r="B43" s="7"/>
       <c r="C43" s="9"/>
     </row>
-    <row r="44" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="44" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="s">
         <v>38</v>
       </c>
@@ -3765,7 +4095,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="45" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="45" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="s">
         <v>39</v>
       </c>
@@ -3774,7 +4104,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="46" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="46" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
         <v>40</v>
       </c>
@@ -3783,7 +4113,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="47" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="47" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
         <v>41</v>
       </c>
@@ -3792,7 +4122,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="48" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="48" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
         <v>42</v>
       </c>
@@ -3801,7 +4131,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="49" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="49" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
         <v>43</v>
       </c>
@@ -3810,7 +4140,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="50" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="50" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>44</v>
       </c>
@@ -3819,7 +4149,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="51" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="51" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A51" s="12" t="s">
         <v>45</v>
       </c>
@@ -3828,7 +4158,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="52" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="52" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="s">
         <v>48</v>
       </c>
@@ -3837,7 +4167,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="53" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="53" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A53" s="12" t="s">
         <v>46</v>
       </c>
@@ -3846,7 +4176,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="54" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="54" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A54" s="12" t="s">
         <v>47</v>
       </c>
@@ -3855,7 +4185,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="55" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="55" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A55" s="12" t="s">
         <v>49</v>
       </c>
@@ -3864,7 +4194,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="56" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="56" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A56" s="12" t="s">
         <v>50</v>
       </c>
@@ -3873,7 +4203,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="57" spans="1:3" s="2" customFormat="1" ht="12">
+    <row r="57" spans="1:3" s="2" customFormat="1" ht="12" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
         <v>51</v>
       </c>
@@ -3882,7 +4212,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="14" t="s">
         <v>7</v>
       </c>
@@ -3891,7 +4221,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="12" customHeight="1">
+    <row r="59" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="10" t="s">
         <v>73</v>
       </c>
@@ -3900,7 +4230,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="12" customHeight="1">
+    <row r="60" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="12" t="s">
         <v>52</v>
       </c>
@@ -3909,7 +4239,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="12" customHeight="1">
+    <row r="61" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="12" t="s">
         <v>53</v>
       </c>
@@ -3918,7 +4248,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="12" customHeight="1">
+    <row r="62" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="12" t="s">
         <v>54</v>
       </c>
@@ -3927,7 +4257,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="12" customHeight="1">
+    <row r="63" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="12" t="s">
         <v>55</v>
       </c>
@@ -3936,7 +4266,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="12" customHeight="1">
+    <row r="64" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="12" t="s">
         <v>56</v>
       </c>
@@ -3945,7 +4275,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="14" t="s">
         <v>8</v>
       </c>
@@ -3954,7 +4284,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="12" customHeight="1">
+    <row r="66" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="10" t="s">
         <v>57</v>
       </c>
@@ -3962,7 +4292,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="12" customHeight="1">
+    <row r="67" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="10" t="s">
         <v>58</v>
       </c>
@@ -3970,7 +4300,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="12" customHeight="1">
+    <row r="68" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="10" t="s">
         <v>59</v>
       </c>
@@ -3978,7 +4308,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="12" customHeight="1">
+    <row r="69" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="10" t="s">
         <v>60</v>
       </c>
@@ -3986,52 +4316,203 @@
         <v>144</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
-      <c r="A70" s="10"/>
-      <c r="C70" s="3"/>
-    </row>
-    <row r="71" spans="1:3">
-      <c r="A71" s="10"/>
-      <c r="C71" s="3"/>
-    </row>
-    <row r="72" spans="1:3">
-      <c r="A72" s="10"/>
-      <c r="C72" s="3"/>
-    </row>
-    <row r="73" spans="1:3">
-      <c r="A73" s="10"/>
-      <c r="C73" s="3"/>
-    </row>
-    <row r="74" spans="1:3">
-      <c r="A74" s="10"/>
-      <c r="C74" s="3"/>
-    </row>
-    <row r="75" spans="1:3">
-      <c r="C75" s="3"/>
-    </row>
-    <row r="76" spans="1:3">
-      <c r="C76" s="3"/>
-    </row>
-    <row r="77" spans="1:3">
+    <row r="70" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B70" s="7"/>
+      <c r="C70" s="9"/>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="10" t="s">
+        <v>331</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="10" t="s">
+        <v>332</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B73" s="45">
+        <v>43101</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B74" s="45">
+        <v>43115</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B75" s="45">
+        <v>43132</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="13" t="s">
+        <v>334</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="13" t="s">
+        <v>336</v>
+      </c>
+      <c r="B77" s="1">
+        <v>330001234</v>
+      </c>
       <c r="C77" s="3"/>
     </row>
-    <row r="78" spans="1:3">
-      <c r="C78" s="3"/>
-    </row>
-    <row r="79" spans="1:3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="13" t="s">
+        <v>337</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="13" t="s">
+        <v>339</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>340</v>
+      </c>
       <c r="C79" s="3"/>
     </row>
-    <row r="80" spans="1:3">
-      <c r="C80" s="3"/>
-    </row>
-    <row r="81" spans="3:3" s="1" customFormat="1">
-      <c r="C81" s="3"/>
-    </row>
-    <row r="82" spans="3:3" s="1" customFormat="1">
-      <c r="C82" s="3"/>
-    </row>
-    <row r="83" spans="3:3" s="1" customFormat="1">
-      <c r="C83" s="3"/>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="13" t="s">
+        <v>341</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="13" t="s">
+        <v>343</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="13" t="s">
+        <v>351</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="13" t="s">
+        <v>353</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="13" t="s">
+        <v>355</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>380</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>